<commit_message>
Broke out caster wheels.
Made the caster assemblies flexible and regen'd SimMechanics files.
This should allow the wheels to turn independently. Also deleted old
urdf file.
</commit_message>
<xml_diff>
--- a/timeline.xlsx
+++ b/timeline.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
@@ -36,15 +36,6 @@
     <t>ROS Gateway</t>
   </si>
   <si>
-    <t>Get IRB-120 Model in Simulator</t>
-  </si>
-  <si>
-    <t>Get ROS Arm Control Working in Simulator</t>
-  </si>
-  <si>
-    <t>Reverse Engineer ABB Control</t>
-  </si>
-  <si>
     <t>Mobility</t>
   </si>
   <si>
@@ -54,19 +45,28 @@
     <t>Week Ending In:</t>
   </si>
   <si>
-    <t>Test Driving by Remote Control</t>
-  </si>
-  <si>
     <t>Reflexive Halt +</t>
   </si>
   <si>
     <t>Order Parts</t>
   </si>
   <si>
-    <t>Fabricate E-Stop Boards</t>
-  </si>
-  <si>
     <t>Rapid</t>
+  </si>
+  <si>
+    <t>Get IRB 120 Model in Simulator</t>
+  </si>
+  <si>
+    <t>Driving by Remote Control (ROS Bringup)</t>
+  </si>
+  <si>
+    <t>Reverse-Engineer ABB Protocol</t>
+  </si>
+  <si>
+    <t>Rapid Stub</t>
+  </si>
+  <si>
+    <t>ROS Arm Control</t>
   </si>
 </sst>
 </file>
@@ -250,13 +250,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -603,25 +606,24 @@
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B5" sqref="B5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="3">
         <v>41019</v>
@@ -682,86 +684,84 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="10"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="11"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="13"/>
+      <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="14"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="20"/>
+      <c r="I4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="8"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -773,23 +773,23 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="7"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -800,21 +800,36 @@
       <c r="T5" s="1"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="H5:I5"/>
+  <mergeCells count="11">
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
     <mergeCell ref="G2:T3"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="E2:E3"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="G4:I4"/>
     <mergeCell ref="J4:L4"/>
-    <mergeCell ref="C2:C3"/>
     <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="B5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>